<commit_message>
Fix Prob of 1 calc. for Sim. Annealing Calc.
</commit_message>
<xml_diff>
--- a/04 - Exams/Final Exam/Scratch Work.xlsx
+++ b/04 - Exams/Final Exam/Scratch Work.xlsx
@@ -6930,7 +6930,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9E231-3205-4664-A989-90DE24B2A06E}">
   <dimension ref="B2:I40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6988,7 +6990,7 @@
         <v xml:space="preserve">1*x1 + </v>
       </c>
       <c r="D6" s="19" t="str">
-        <f t="shared" ref="D6:G6" si="1">D5 &amp; "*" &amp; D9 &amp; " + "</f>
+        <f t="shared" ref="D6:F6" si="1">D5 &amp; "*" &amp; D9 &amp; " + "</f>
         <v xml:space="preserve">2*x2 + </v>
       </c>
       <c r="E6" s="19" t="str">
@@ -7149,7 +7151,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="67">
-        <f t="shared" ref="H11:H13" si="4">SUMPRODUCT(C13:G13, C$5:G$5)</f>
+        <f t="shared" ref="H13" si="4">SUMPRODUCT(C13:G13, C$5:G$5)</f>
         <v>3</v>
       </c>
       <c r="I13" s="72" t="str">

</xml_diff>